<commit_message>
Update contents for electricity data Excel workbook
</commit_message>
<xml_diff>
--- a/data/electricity_clean.xlsx
+++ b/data/electricity_clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robyn/PycharmProjects/bdc/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robyn/PycharmProjects/cfg-big-data-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B164F6-7E78-734F-AB96-ABA5B08C9762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E4FA8F-B794-F145-AC4E-6652E3A8686D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23300" yWindow="460" windowWidth="15100" windowHeight="19540" firstSheet="17" activeTab="19" xr2:uid="{D3D9E6EF-7CDD-2D4C-979A-3E58E75DD25C}"/>
+    <workbookView xWindow="23300" yWindow="460" windowWidth="15100" windowHeight="19540" xr2:uid="{D3D9E6EF-7CDD-2D4C-979A-3E58E75DD25C}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="81">
   <si>
     <t>coal</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Timescale</t>
   </si>
   <si>
-    <t>Supply</t>
-  </si>
-  <si>
     <t xml:space="preserve">Electricity available (TWh) in the distribution system from all UK generation, imports and other sources. </t>
   </si>
   <si>
@@ -266,9 +263,6 @@
   </si>
   <si>
     <t>Monthly</t>
-  </si>
-  <si>
-    <t>Demand</t>
   </si>
   <si>
     <t>Electricity sold (TWh)</t>
@@ -305,6 +299,9 @@
   </si>
   <si>
     <t>renewable</t>
+  </si>
+  <si>
+    <t>Annually</t>
   </si>
 </sst>
 </file>
@@ -524,10 +521,10 @@
       <sheetName val="Calculation"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4">
         <row r="4">
           <cell r="C4" t="str">
@@ -2862,8 +2859,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3166,195 +3163,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFC29EB-9B4F-DD45-814A-1F378276BC8C}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="90.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>12</v>
       </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
       <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2">
+        <v>65</v>
+      </c>
+      <c r="D2">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1.2</v>
       </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3">
+        <v>65</v>
+      </c>
+      <c r="D3">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1.3</v>
       </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
       <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4">
+        <v>65</v>
+      </c>
+      <c r="D4">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>2.1</v>
       </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5">
+        <v>65</v>
+      </c>
+      <c r="D5">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2.2000000000000002</v>
       </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6">
+        <v>65</v>
+      </c>
+      <c r="D6">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2.2999999999999998</v>
       </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7">
+        <v>65</v>
+      </c>
+      <c r="D7">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>3.1</v>
       </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
       <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8">
+        <v>65</v>
+      </c>
+      <c r="D8">
         <v>5.2</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>3.2</v>
       </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
       <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9">
+        <v>65</v>
+      </c>
+      <c r="D9">
         <v>5.2</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>3.3</v>
       </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
       <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10">
+        <v>65</v>
+      </c>
+      <c r="D10">
         <v>5.2</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>3.4</v>
       </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
       <c r="C11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11">
+        <v>65</v>
+      </c>
+      <c r="D11">
         <v>5.2</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>4.0999999999999996</v>
       </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
       <c r="C12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12">
+        <v>80</v>
+      </c>
+      <c r="D12">
         <v>5.3</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>4.2</v>
       </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
       <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13">
+        <v>65</v>
+      </c>
+      <c r="D13">
         <v>5.3</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>4.3</v>
       </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
       <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14">
+        <v>67</v>
+      </c>
+      <c r="D14">
         <v>5.3</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>5.0999999999999996</v>
       </c>
@@ -3364,17 +3400,14 @@
       <c r="C15" t="s">
         <v>65</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15">
+        <v>5.5</v>
+      </c>
+      <c r="E15" t="s">
         <v>66</v>
       </c>
-      <c r="E15">
-        <v>5.5</v>
-      </c>
-      <c r="F15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>5.2</v>
       </c>
@@ -3382,53 +3415,44 @@
         <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16">
+        <v>67</v>
+      </c>
+      <c r="D16">
         <v>5.5</v>
       </c>
-      <c r="F16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>6.1</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17">
+        <v>65</v>
+      </c>
+      <c r="D17">
         <v>5.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>6.2</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18">
+        <v>67</v>
+      </c>
+      <c r="D18">
         <v>5.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>7.1</v>
       </c>
@@ -3436,19 +3460,16 @@
         <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19">
+        <v>65</v>
+      </c>
+      <c r="D19">
         <v>5.5</v>
       </c>
-      <c r="F19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="E19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>7.2</v>
       </c>
@@ -3456,83 +3477,68 @@
         <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20">
+        <v>67</v>
+      </c>
+      <c r="D20">
         <v>5.5</v>
       </c>
-      <c r="F20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>8.1</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21">
+        <v>65</v>
+      </c>
+      <c r="D21">
         <v>5.4</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>8.1999999999999993</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22">
+        <v>67</v>
+      </c>
+      <c r="D22">
         <v>5.4</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>9.1</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23">
+        <v>65</v>
+      </c>
+      <c r="D23">
         <v>5.4</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>9.1999999999999993</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24">
+        <v>67</v>
+      </c>
+      <c r="D24">
         <v>5.4</v>
       </c>
     </row>
@@ -24254,7 +24260,7 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -25407,7 +25413,7 @@
         <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -28804,7 +28810,7 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -29957,7 +29963,7 @@
         <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -33356,13 +33362,13 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
         <v>77</v>
-      </c>
-      <c r="D1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -35109,7 +35115,7 @@
   <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -38818,8 +38824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970DEB5E-50F3-5446-8CFE-E566FCB56113}">
   <dimension ref="A1:E307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B33" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -38839,13 +38845,13 @@
         <v>62</v>
       </c>
       <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
         <v>77</v>
-      </c>
-      <c r="D1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -44079,10 +44085,10 @@
         <v>11</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -45428,10 +45434,10 @@
         <v>62</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>

<commit_message>
Correct non-renewable/renewable to fossil/non-fossil
</commit_message>
<xml_diff>
--- a/data/electricity_clean.xlsx
+++ b/data/electricity_clean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robyn/PycharmProjects/cfg-big-data-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E4FA8F-B794-F145-AC4E-6652E3A8686D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19B2C5C-5C95-DD44-A982-C6874CA4AD7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23300" yWindow="460" windowWidth="15100" windowHeight="19540" xr2:uid="{D3D9E6EF-7CDD-2D4C-979A-3E58E75DD25C}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2034" uniqueCount="82">
   <si>
     <t>coal</t>
   </si>
@@ -295,13 +295,16 @@
     <t>electricity_sold_other</t>
   </si>
   <si>
-    <t>non-renewable</t>
+    <t>Annually</t>
   </si>
   <si>
-    <t>renewable</t>
+    <t>This is actually fossil vs non-fossil fuels as nuclear is included in renewable but it isn't technically classed as renewable energy</t>
   </si>
   <si>
-    <t>Annually</t>
+    <t>fossil</t>
+  </si>
+  <si>
+    <t>non-fossil</t>
   </si>
 </sst>
 </file>
@@ -3166,7 +3169,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3174,6 +3177,7 @@
     <col min="2" max="2" width="90.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="188.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3353,7 +3357,7 @@
         <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D12">
         <v>5.3</v>
@@ -3499,6 +3503,9 @@
       <c r="D21">
         <v>5.4</v>
       </c>
+      <c r="E21" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
@@ -3512,6 +3519,9 @@
       </c>
       <c r="D22">
         <v>5.4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -5915,7 +5925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB00411D-A5C1-2242-9AA1-61BE32DAD4AB}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -44066,7 +44076,7 @@
   <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -44085,10 +44095,10 @@
         <v>11</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -45417,7 +45427,7 @@
   <dimension ref="A1:D283"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -45434,10 +45444,10 @@
         <v>62</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>

<commit_message>
Clean month column on worksheet 5.2
</commit_message>
<xml_diff>
--- a/data/electricity_clean.xlsx
+++ b/data/electricity_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robyn/PycharmProjects/cfg-big-data-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED2EA7F-E241-6243-BB5B-360BF0F183ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E5CD68-4AE8-8B4C-B241-E5EA774990FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23300" yWindow="460" windowWidth="15100" windowHeight="19540" xr2:uid="{D3D9E6EF-7CDD-2D4C-979A-3E58E75DD25C}"/>
+    <workbookView xWindow="20200" yWindow="460" windowWidth="18200" windowHeight="19540" xr2:uid="{D3D9E6EF-7CDD-2D4C-979A-3E58E75DD25C}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -3184,7 +3184,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3420,7 +3420,7 @@
         <v>65</v>
       </c>
       <c r="D15">
-        <v>5.5</v>
+        <v>5.4</v>
       </c>
       <c r="E15" t="s">
         <v>66</v>
@@ -3437,7 +3437,7 @@
         <v>67</v>
       </c>
       <c r="D16">
-        <v>5.5</v>
+        <v>5.4</v>
       </c>
       <c r="E16" t="s">
         <v>66</v>
@@ -25434,7 +25434,7 @@
   <dimension ref="A1:C307"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -26142,7 +26142,7 @@
         <v>2000</v>
       </c>
       <c r="B64" s="55" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C64" s="56">
         <v>33.506999999999998</v>
@@ -28012,7 +28012,7 @@
         <v>2014</v>
       </c>
       <c r="B234" s="55" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C234" s="57">
         <v>25.032112687202414</v>

</xml_diff>

<commit_message>
Update renewable and non-renewable groupings
</commit_message>
<xml_diff>
--- a/data/electricity_clean.xlsx
+++ b/data/electricity_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robyn/PycharmProjects/cfg-big-data-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC7A2E0-10D1-3F44-B8D5-D3282C87FA26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635DA8AC-EE8F-C640-8D2F-B07510743AC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20200" yWindow="460" windowWidth="18200" windowHeight="19540" firstSheet="16" activeTab="22" xr2:uid="{D3D9E6EF-7CDD-2D4C-979A-3E58E75DD25C}"/>
+    <workbookView xWindow="20200" yWindow="460" windowWidth="18200" windowHeight="19540" xr2:uid="{D3D9E6EF-7CDD-2D4C-979A-3E58E75DD25C}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -3183,8 +3183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFC29EB-9B4F-DD45-814A-1F378276BC8C}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -46056,8 +46056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55480FB2-8C6B-5C42-9FA3-459C4F024B62}">
   <dimension ref="A1:D283"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -46693,7 +46693,7 @@
         <v>2000</v>
       </c>
       <c r="B40" s="55" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C40" s="52">
         <f>SUM('9.2'!C40:F40,'9.2'!K40)</f>
@@ -53953,8 +53953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BF825A-D0FA-8F40-AE34-FAE0B0C8E26D}">
   <dimension ref="A1:K283"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A215" workbookViewId="0">
+      <selection activeCell="B260" sqref="B260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>